<commit_message>
[doc] script (java script)
</commit_message>
<xml_diff>
--- a/doc/study.xlsx
+++ b/doc/study.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48FC3CD-4D60-41F6-A6F3-AE60A86EDBEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-5700" windowWidth="25440" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-5700" windowWidth="25440" windowHeight="15990" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
     <sheet name="put main image" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="script" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>No</t>
   </si>
@@ -30,12 +30,21 @@
   <si>
     <t>index!A1</t>
   </si>
+  <si>
+    <t>script</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/tags/tag_script.asp</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,7 +148,7 @@
         <xdr:cNvPr id="2049" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -192,7 +201,7 @@
         <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -240,7 +249,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -303,7 +312,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -356,7 +365,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -409,7 +418,7 @@
         <xdr:cNvPr id="9" name="Oval 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -475,7 +484,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -528,7 +537,7 @@
         <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -581,7 +590,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -634,7 +643,7 @@
         <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -682,7 +691,7 @@
         <xdr:cNvPr id="15" name="TextBox 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -747,7 +756,7 @@
         <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -805,7 +814,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ADDD7B4-6DC4-4AEE-A2CC-BF3B4F824717}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3ADDD7B4-6DC4-4AEE-A2CC-BF3B4F824717}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -817,7 +826,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -855,7 +864,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8F85461-69A0-4810-87B5-EA7399038BA0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8F85461-69A0-4810-87B5-EA7399038BA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -867,7 +876,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -905,7 +914,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79DA0762-A853-4EC5-AFA9-8A97437355B3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79DA0762-A853-4EC5-AFA9-8A97437355B3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -940,6 +949,406 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2049" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="762000"/>
+          <a:ext cx="13992225" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1457325" y="1476375"/>
+          <a:ext cx="1733550" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="3124201" y="1390649"/>
+          <a:ext cx="5953125" cy="1438275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2122184" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2390775" y="2952750"/>
+          <a:ext cx="2122184" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>what does this mean? java</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> script?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>278332</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2050" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="887932" y="3476625"/>
+          <a:ext cx="7094018" cy="3048000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6038850" y="2886075"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4714875" y="3267075"/>
+          <a:ext cx="3524250" cy="1790700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1327351" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 13"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8448675" y="5010150"/>
+          <a:ext cx="1327351" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>should be javascript</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -986,7 +1395,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1018,27 +1427,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1070,24 +1461,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1263,20 +1636,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:C26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="5.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1284,7 +1657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -1292,122 +1665,125 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3">
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3">
       <c r="B7" s="2">
         <v>3</v>
       </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
       <c r="B8" s="2">
         <v>4</v>
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3">
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3">
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3">
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3">
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3">
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3">
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3">
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3">
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3">
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3">
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3">
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3">
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3">
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3">
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3">
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3">
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3">
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3">
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" location="'put main image'!A1" display="Put main image" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C5" location="'put main image'!A1" display="Put main image"/>
+    <hyperlink ref="C7" location="script!A1" display="script"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Z48" sqref="Z48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="index!A1" display="index!A1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A1" location="index!A1" display="index!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1415,16 +1791,48 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S36" sqref="S36"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B36"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="index!A1" display="index!A1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[doc] class, web map
</commit_message>
<xml_diff>
--- a/doc/study.xlsx
+++ b/doc/study.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885A25E3-B67F-454F-B5CB-712F4EBA9F37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -13,13 +12,15 @@
     <sheet name="Link html" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
     <sheet name="script" sheetId="4" r:id="rId5"/>
+    <sheet name="class" sheetId="6" r:id="rId6"/>
+    <sheet name="web map" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>No</t>
   </si>
@@ -41,12 +42,18 @@
   <si>
     <t>https://www.w3schools.com/tags/tag_script.asp</t>
   </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>web  map</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,7 +157,7 @@
         <xdr:cNvPr id="2049" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -203,7 +210,7 @@
         <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -251,7 +258,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -314,7 +321,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -367,7 +374,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -420,7 +427,7 @@
         <xdr:cNvPr id="9" name="Oval 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -486,7 +493,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -539,7 +546,7 @@
         <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -592,7 +599,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -645,7 +652,7 @@
         <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -693,7 +700,7 @@
         <xdr:cNvPr id="15" name="TextBox 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -758,7 +765,7 @@
         <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -816,7 +823,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ADDD7B4-6DC4-4AEE-A2CC-BF3B4F824717}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3ADDD7B4-6DC4-4AEE-A2CC-BF3B4F824717}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -828,7 +835,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -866,7 +873,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8F85461-69A0-4810-87B5-EA7399038BA0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8F85461-69A0-4810-87B5-EA7399038BA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -878,7 +885,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -916,7 +923,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79DA0762-A853-4EC5-AFA9-8A97437355B3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79DA0762-A853-4EC5-AFA9-8A97437355B3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -974,7 +981,7 @@
         <xdr:cNvPr id="2049" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1027,7 +1034,7 @@
         <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1080,7 +1087,7 @@
         <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1128,7 +1135,7 @@
         <xdr:cNvPr id="7" name="TextBox 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1198,7 +1205,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1246,7 +1253,7 @@
         <xdr:cNvPr id="11" name="TextBox 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1306,7 +1313,7 @@
         <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1354,7 +1361,7 @@
         <xdr:cNvPr id="14" name="TextBox 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1399,6 +1406,926 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="571500"/>
+          <a:ext cx="4200525" cy="4143375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1266825" y="762000"/>
+          <a:ext cx="3314700" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="808363" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4876800" y="714375"/>
+          <a:ext cx="808363" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>nama class</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>536575</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Freeform 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1285875" y="869950"/>
+          <a:ext cx="1079500" cy="1787525"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 704850 w 1079500"/>
+            <a:gd name="connsiteY0" fmla="*/ 1787525 h 1787525"/>
+            <a:gd name="connsiteX1" fmla="*/ 962025 w 1079500"/>
+            <a:gd name="connsiteY1" fmla="*/ 292100 h 1787525"/>
+            <a:gd name="connsiteX2" fmla="*/ 0 w 1079500"/>
+            <a:gd name="connsiteY2" fmla="*/ 34925 h 1787525"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="1079500" h="1787525">
+              <a:moveTo>
+                <a:pt x="704850" y="1787525"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="892175" y="1185862"/>
+                <a:pt x="1079500" y="584200"/>
+                <a:pt x="962025" y="292100"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="844550" y="0"/>
+                <a:pt x="422275" y="17462"/>
+                <a:pt x="0" y="34925"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:ln>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1153906" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2295525" y="2019300"/>
+          <a:ext cx="1153906" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>merefensi ke sini</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>335272</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2049" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="944872" y="895350"/>
+          <a:ext cx="14819003" cy="7467600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>56030</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Oval 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8650941" y="1109382"/>
+          <a:ext cx="1086971" cy="1669677"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>515470</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>369795</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9592235" y="1647265"/>
+          <a:ext cx="7115736" cy="358588"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>89647</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>123265</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Oval 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="694765" y="2420471"/>
+          <a:ext cx="15766676" cy="705970"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="568297" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16943294" y="1972235"/>
+          <a:ext cx="568297" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>iki opo</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>186018</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>163605</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="568297" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17129312" y="2640105"/>
+          <a:ext cx="568297" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>iki opo</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>302559</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>33618</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="16640735" y="2801471"/>
+          <a:ext cx="336177" cy="56029"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>369794</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>56030</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Oval 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8841441" y="4919382"/>
+          <a:ext cx="896471" cy="526677"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>168088</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>33619</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>112059</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Oval 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="773206" y="3462619"/>
+          <a:ext cx="15677029" cy="1680882"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>537883</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>145678</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="16142074" y="3098427"/>
+          <a:ext cx="1075765" cy="818030"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>156882</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>549088</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Oval 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="750794"/>
+          <a:ext cx="14915029" cy="437030"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15508941" y="1019735"/>
+          <a:ext cx="1423147" cy="930089"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1445,7 +2372,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1477,27 +2404,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1529,24 +2438,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1722,20 +2613,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:C26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="5.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1743,7 +2634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -1751,13 +2642,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3">
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3">
       <c r="B7" s="2">
         <v>3</v>
       </c>
@@ -1765,111 +2656,119 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3">
       <c r="B8" s="2">
         <v>4</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
+    <row r="9" spans="2:3">
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3">
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3">
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3">
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3">
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3">
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3">
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3">
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3">
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3">
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3">
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3">
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3">
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3">
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3">
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3">
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3">
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3">
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" location="'put main image'!A1" display="Put main image" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C7" location="script!A1" display="script" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C5" location="'put main image'!A1" display="Put main image"/>
+    <hyperlink ref="C7" location="script!A1" display="script"/>
+    <hyperlink ref="C8" location="class!A1" display="class"/>
+    <hyperlink ref="C9" location="'web map'!A1" display="web  map"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Z48" sqref="Z48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="index!A1" display="index!A1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A1" location="index!A1" display="index!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1877,26 +2776,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46E415D-B15E-44CB-956C-2B6BB3ABEBD2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1904,21 +2803,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1928,7 +2827,53 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="index!A1" display="index!A1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="A1" location="index!A1" display="index!A1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="index!A1" display="index!A1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="index!A1" display="index!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>